<commit_message>
before fix nhap_hang case >=12
</commit_message>
<xml_diff>
--- a/public/uploads/nhap_hang_sapo.xlsx
+++ b/public/uploads/nhap_hang_sapo.xlsx
@@ -580,7 +580,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="221">
   <si>
     <t>Mã đơn nhập</t>
   </si>
@@ -657,328 +657,592 @@
     <t>Ngày hết hạn</t>
   </si>
   <si>
-    <t>ASAMBAOGCWCBLACK-38</t>
-  </si>
-  <si>
-    <t>Giày Adidas Samba OG Cloud White Core Black Samba Trắng Logo Đen Mũi Xám - Size 38</t>
-  </si>
-  <si>
-    <t>ASAMBAOGCWCBLACK-40</t>
-  </si>
-  <si>
-    <t>Giày Adidas Samba OG Cloud White Core Black Samba Trắng Logo Đen Mũi Xám - Size 40</t>
-  </si>
-  <si>
-    <t>ASAMBAOGCWCBLACK-43</t>
-  </si>
-  <si>
-    <t>Giày Adidas Samba OG Cloud White Core Black Samba Trắng Logo Đen Mũi Xám - Size 43</t>
-  </si>
-  <si>
-    <t>AYMXOAT-38</t>
-  </si>
-  <si>
-    <t>Giày Adidas Yeezy 350 V2 MX Oat Kem Loang Hàng Đế Nén Hạt Chuẩn - Size 38</t>
-  </si>
-  <si>
-    <t>AYMXOAT-39</t>
-  </si>
-  <si>
-    <t>Giày Adidas Yeezy 350 V2 MX Oat Kem Loang Hàng Đế Nén Hạt Chuẩn - Size 39</t>
-  </si>
-  <si>
-    <t>AYMXOAT-41</t>
-  </si>
-  <si>
-    <t>Giày Adidas Yeezy 350 V2 MX Oat Kem Loang Hàng Đế Nén Hạt Chuẩn - Size 41</t>
-  </si>
-  <si>
-    <t>AYMXOAT-45</t>
-  </si>
-  <si>
-    <t>Giày Adidas Yeezy 350 V2 MX Oat Kem Loang Hàng Đế Nén Hạt Chuẩn - Size 45</t>
-  </si>
-  <si>
-    <t>AYMXOAT-42</t>
-  </si>
-  <si>
-    <t>Giày Adidas Yeezy 350 V2 MX Oat Kem Loang Hàng Đế Nén Hạt Chuẩn - Size 42</t>
-  </si>
-  <si>
-    <t>NAF1CHAMPSC-40</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Force 1 Reigning Champ Xám Da Lộn - Size 40</t>
-  </si>
-  <si>
-    <t>NAF1CHAMPSC-41</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Force 1 Reigning Champ Xám Da Lộn - Size 41</t>
-  </si>
-  <si>
-    <t>NAF1CHAMPSC-42</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Force 1 Reigning Champ Xám Da Lộn - Size 42</t>
-  </si>
-  <si>
-    <t>NAF1CHAMPSC-45</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Force 1 Reigning Champ Xám Da Lộn - Size 45</t>
-  </si>
-  <si>
-    <t>NAF1PICANTE-38</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Force 1 White Picante Trắng Xám - Size 38</t>
-  </si>
-  <si>
-    <t>NAF1PICANTE-39</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Force 1 White Picante Trắng Xám - Size 39</t>
-  </si>
-  <si>
-    <t>NAF1PICANTE-40</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Force 1 White Picante Trắng Xám - Size 40</t>
-  </si>
-  <si>
-    <t>NAF1PICANTE-41</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Force 1 White Picante Trắng Xám - Size 41</t>
-  </si>
-  <si>
-    <t>NAF1PICANTE-42</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Force 1 White Picante Trắng Xám - Size 42</t>
-  </si>
-  <si>
-    <t>NAF1PICANTE-43</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Force 1 White Picante Trắng Xám - Size 43</t>
-  </si>
-  <si>
-    <t>NAF1PICANTE-44</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Force 1 White Picante Trắng Xám - Size 44</t>
-  </si>
-  <si>
-    <t>NAF1PICANTE-45</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Force 1 White Picante Trắng Xám - Size 45</t>
-  </si>
-  <si>
-    <t>NJD1CROGLOLLEN-40</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 1 High Retro OG Pollen, JD1 Cao Vàng Đen - Size 40</t>
-  </si>
-  <si>
-    <t>NJD1CROGLOLLEN-41</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 1 High Retro OG Pollen, JD1 Cao Vàng Đen - Size 41</t>
-  </si>
-  <si>
-    <t>NJD1CROGLOLLEN-43</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 1 High Retro OG Pollen, JD1 Cao Vàng Đen - Size 43</t>
-  </si>
-  <si>
-    <t>NJD1CROGLOLLEN-45</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 1 High Retro OG Pollen, JD1 Cao Vàng Đen - Size 45</t>
-  </si>
-  <si>
-    <t>NJD1CROGLOLLEN-42</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 1 High Retro OG Pollen, JD1 Cao Vàng Đen - Size 42</t>
-  </si>
-  <si>
-    <t>NJD4KAWSBLACK-40</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 4 Kaws Black, JD4 Đen Full Da Lộn Đế Dạ Quang - Size 40</t>
-  </si>
-  <si>
-    <t>NJD4KAWSBLACK-41</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 4 Kaws Black, JD4 Đen Full Da Lộn Đế Dạ Quang - Size 41</t>
-  </si>
-  <si>
-    <t>NJD4KAWSBLACK-43</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 4 Kaws Black, JD4 Đen Full Da Lộn Đế Dạ Quang - Size 43</t>
-  </si>
-  <si>
-    <t>NJD4KAWSBLACK-42</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 4 Kaws Black, JD4 Đen Full Da Lộn Đế Dạ Quang - Size 42</t>
-  </si>
-  <si>
-    <t>NJD4RBLACKCAT-41</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 4 Retro Black Cat, JD4 Đen Full - Size 41</t>
-  </si>
-  <si>
-    <t>NJD4RBLACKCAT-43</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 4 Retro Black Cat, JD4 Đen Full - Size 43</t>
-  </si>
-  <si>
-    <t>NJD4RBLACKCAT-45</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 4 Retro Black Cat, JD4 Đen Full - Size 45</t>
-  </si>
-  <si>
-    <t>NJD4TFIRERED-38</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 4 Fire Red, JD4 Trắng Viền Đỏ - Size 38</t>
-  </si>
-  <si>
-    <t>NJD4TFIRERED-44</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 4 Fire Red, JD4 Trắng Viền Đỏ - Size 44</t>
-  </si>
-  <si>
-    <t>NJD4TFIRERED-45</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 4 Fire Red, JD4 Trắng Viền Đỏ - Size 45</t>
-  </si>
-  <si>
-    <t>NJD4TFIRERED-42</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 4 Fire Red, JD4 Trắng Viền Đỏ - Size 42</t>
-  </si>
-  <si>
-    <t>NJD4TFIRERED-41</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 4 Fire Red, JD4 Trắng Viền Đỏ - Size 41</t>
-  </si>
-  <si>
-    <t>NMAX270DSGR-39</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Max 270 Pulse Roam Dark Smoke Grey Đen Xám Navy - Size 39</t>
-  </si>
-  <si>
-    <t>NMAX270DSGR-40</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Max 270 Pulse Roam Dark Smoke Grey Đen Xám Navy - Size 40</t>
-  </si>
-  <si>
-    <t>NMAX270DSGR-41</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Max 270 Pulse Roam Dark Smoke Grey Đen Xám Navy - Size 41</t>
-  </si>
-  <si>
-    <t>NMAX270DSGR-42</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Max 270 Pulse Roam Dark Smoke Grey Đen Xám Navy - Size 42</t>
-  </si>
-  <si>
-    <t>NSBLWN-42</t>
-  </si>
-  <si>
-    <t>Giày Nike SB Dunk Low Orange Label White Navy, SB Trắng Đế Nâu - Size 42</t>
-  </si>
-  <si>
-    <t>NSBLWN-44</t>
-  </si>
-  <si>
-    <t>Giày Nike SB Dunk Low Orange Label White Navy, SB Trắng Đế Nâu - Size 44</t>
-  </si>
-  <si>
-    <t>NZBW-40</t>
-  </si>
-  <si>
-    <t>Giày Nike Zoom Pegasus 35 Turbo 2.0 Black White, Zoom Đen Trắng - Size 40</t>
-  </si>
-  <si>
-    <t>NZBW-41</t>
-  </si>
-  <si>
-    <t>Giày Nike Zoom Pegasus 35 Turbo 2.0 Black White, Zoom Đen Trắng - Size 41</t>
-  </si>
-  <si>
-    <t>NZBW-42</t>
-  </si>
-  <si>
-    <t>Giày Nike Zoom Pegasus 35 Turbo 2.0 Black White, Zoom Đen Trắng - Size 42</t>
-  </si>
-  <si>
-    <t>NZBW-43</t>
-  </si>
-  <si>
-    <t>Giày Nike Zoom Pegasus 35 Turbo 2.0 Black White, Zoom Đen Trắng - Size 43</t>
-  </si>
-  <si>
-    <t>VANSKNUWBLACK-40</t>
-  </si>
-  <si>
-    <t>Giày Vans Knu Skool Black White Đen Trắng - Size 40</t>
-  </si>
-  <si>
-    <t>VANSKNUWBLACK-41</t>
-  </si>
-  <si>
-    <t>Giày Vans Knu Skool Black White Đen Trắng - Size 41</t>
-  </si>
-  <si>
-    <t>VANSKNUWBLACK-42</t>
-  </si>
-  <si>
-    <t>Giày Vans Knu Skool Black White Đen Trắng - Size 42</t>
-  </si>
-  <si>
-    <t>VANSKNUWHTE-39</t>
-  </si>
-  <si>
-    <t>Giày Vans Knu Skool True White Leather Full Trắng - Size 39</t>
-  </si>
-  <si>
-    <t>VANSKNUWHTE-40</t>
-  </si>
-  <si>
-    <t>Giày Vans Knu Skool True White Leather Full Trắng - Size 40</t>
-  </si>
-  <si>
-    <t>VANSKNUWHTE-42</t>
-  </si>
-  <si>
-    <t>Giày Vans Knu Skool True White Leather Full Trắng - Size 42</t>
-  </si>
-  <si>
-    <t>VANSKNUWHTE-41</t>
-  </si>
-  <si>
-    <t>Giày Vans Knu Skool True White Leather Full Trắng - Size 41</t>
+    <t>AKILLSHOT2LGR</t>
+  </si>
+  <si>
+    <t>Giày Nike KillShot 2 Lucid Green Xanh Lá Xám Da Lộn</t>
+  </si>
+  <si>
+    <t>AKILLSHOT2SAGU</t>
+  </si>
+  <si>
+    <t>Giày Nike KillShot 2 Sail Gum Trắng Xám Da Lộn</t>
+  </si>
+  <si>
+    <t>APUREBTCARBON</t>
+  </si>
+  <si>
+    <t>Giày Adidas Pureboost Carbon, PureBoost Đen Logo Trắng</t>
+  </si>
+  <si>
+    <t>APUREBWHITEBLACK</t>
+  </si>
+  <si>
+    <t>Giày Adidas Pureboost White Black, PureBoost Trắng Sọc Đen</t>
+  </si>
+  <si>
+    <t>APURETRWHITE</t>
+  </si>
+  <si>
+    <t>Giày Adidas Pureboost Triple White Full Trắng</t>
+  </si>
+  <si>
+    <t>ASAMBAOGCWCBLACK</t>
+  </si>
+  <si>
+    <t>Giày Adidas Samba OG Cloud White Core Black Samba Trắng Logo Đen Mũi Xám</t>
+  </si>
+  <si>
+    <t>ASAMBATWHHH</t>
+  </si>
+  <si>
+    <t>Giày Adidas Samba Pharrell Williams Humanrace Samba Full Kem Da Lộn</t>
+  </si>
+  <si>
+    <t>ASGL</t>
+  </si>
+  <si>
+    <t>Giày Adidas Superstar Gold Label Superstar Tem Vàng</t>
+  </si>
+  <si>
+    <t>AYMXGREY</t>
+  </si>
+  <si>
+    <t>Giày Adidas Yeezy 350 V2 MX Frost Blue Đen Xám Trắng Hàng Đế Nén Hạt Chuẩn</t>
+  </si>
+  <si>
+    <t>AYSLATE</t>
+  </si>
+  <si>
+    <t>Giày Adidas Yeezy 350 V2 Slate Kem Kẻ Đen Hàng Đế Nén Hạt Chuẩn</t>
+  </si>
+  <si>
+    <t>AYZ350BLACKDPQ</t>
+  </si>
+  <si>
+    <t>Giày Adidas Yeezy 350 V2 Black Reflective Đen Phản Quang Boost Nén Hạt</t>
+  </si>
+  <si>
+    <t>AYZ350CINDER</t>
+  </si>
+  <si>
+    <t>Giày Adidas Yeezy 350 V2 Cinder Đen Full</t>
+  </si>
+  <si>
+    <t>AYZ350STATICNONTPQ</t>
+  </si>
+  <si>
+    <t>Giày Adidas Yeezy 350 V2 Static Reflective Trắng Phản Quang Boost Nén Hạt</t>
+  </si>
+  <si>
+    <t>AYZ350V2LUNDMARK</t>
+  </si>
+  <si>
+    <t>Giày Adidas Yeezy 350 V2 Lundmark Reflective Kem Xám Boost Nén Hạt</t>
+  </si>
+  <si>
+    <t>AYZ350V2SESAME</t>
+  </si>
+  <si>
+    <t>Giày Adidas Yeezy 350 V2 Sesame Xám Xi Măng Boost Nén Hạt</t>
+  </si>
+  <si>
+    <t>AYZXCW</t>
+  </si>
+  <si>
+    <t>Giày Adidas Yeezy 350 V2 Cloud White Trắng Xanh</t>
+  </si>
+  <si>
+    <t>MLBCHUNKYWPINK</t>
+  </si>
+  <si>
+    <t>Giày MLB Chunky Liner Denim Monogram NY White Pink Trắng Hồng</t>
+  </si>
+  <si>
+    <t>NAF1BGGUM</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Force 1 Low Beige Green Gum, AF1 Trắng Móc Xanh Đế Nâu</t>
+  </si>
+  <si>
+    <t>NAF1FTSC</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Force 1 Low Triple White, AF1 Full Trắng SC</t>
+  </si>
+  <si>
+    <t>NAF1JUSTDOITHANGTAG</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Force 1 Low Just Do It Hangtag, AF1 Trắng Lòng Đỏ Móc Đồng Xu</t>
+  </si>
+  <si>
+    <t>NAF1LIORBR</t>
+  </si>
+  <si>
+    <t>Giày AF1 Light Orewood Brown Xám Nâu</t>
+  </si>
+  <si>
+    <t>NAF1NYCCOATHLETE</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Force 1 Low NYC City of Athletes, AF1 New York Nhiều Màu</t>
+  </si>
+  <si>
+    <t>NAF1TRIPLEBLACKSC</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Force 1 Triple Black Full Đen</t>
+  </si>
+  <si>
+    <t>NAF1TXDX</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Force 1 Low 07 Cream White Navy Skate, AF1 Trắng Móc Xanh Đế Xanh</t>
+  </si>
+  <si>
+    <t>NAF1WB</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Force 1 Low White Black, AF1 Trắng Móc Đen</t>
+  </si>
+  <si>
+    <t>NAM90BW</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 90 Black White Đen Trắng</t>
+  </si>
+  <si>
+    <t>NAM90JEWEL</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 90 Jewel Wolf Grey Xám</t>
+  </si>
+  <si>
+    <t>NAM90NWB</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 90 Nature White Black Trắng Đen</t>
+  </si>
+  <si>
+    <t>NAM95COGR</t>
+  </si>
+  <si>
+    <t>Giày Max 95 Cool Grey Xám Đậm</t>
+  </si>
+  <si>
+    <t>NAM95FRMI</t>
+  </si>
+  <si>
+    <t>Giày Max 95 Fresh Mint Xám Đen Xanh Lá</t>
+  </si>
+  <si>
+    <t>NAM95TRBL</t>
+  </si>
+  <si>
+    <t>Giày Max 95 Triple Black Full Đen</t>
+  </si>
+  <si>
+    <t>NB2002RMINA</t>
+  </si>
+  <si>
+    <t>Giày New Balance 2002 Midnight Navy Đen Xanh Navy</t>
+  </si>
+  <si>
+    <t>NB2002RRAINCLOUD</t>
+  </si>
+  <si>
+    <t>Giày New Balance 2002R Protection Pack Rain Cloud, NB 2002R Xám Xanh -Than.Shoes</t>
+  </si>
+  <si>
+    <t>NB530ALLBLACK</t>
+  </si>
+  <si>
+    <t>Giày New Balance 530 All Black, NB 530 Đen Logo Trắng</t>
+  </si>
+  <si>
+    <t>NB530GREYMHG</t>
+  </si>
+  <si>
+    <t>Giày New Balance 530 Grey Matter Harbor Grey, NB 530 Xám Da Lộn</t>
+  </si>
+  <si>
+    <t>NB530RRNAVY</t>
+  </si>
+  <si>
+    <t>Giày New Balance 530 Retro Running Navy, NB 530 Xanh Than</t>
+  </si>
+  <si>
+    <t>NB530WHITESILVER</t>
+  </si>
+  <si>
+    <t>Giày New Balance 530 White Silver, NB 530 Trắng Bạc Xám</t>
+  </si>
+  <si>
+    <t>NB740BS</t>
+  </si>
+  <si>
+    <t>Giày New Balance 740 Black Silver Đen Bạc</t>
+  </si>
+  <si>
+    <t>NJD1CBANNED</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 Mid Banned, JD1 Cao Đỏ Đen</t>
+  </si>
+  <si>
+    <t>NJD1CCSCHICAGO</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 Mid GS Chicago, JD1 Cao Trắng Đỏ Móc Đen</t>
+  </si>
+  <si>
+    <t>NJD1CDENIM</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 High Denim Cổ Cao Xanh Jeans</t>
+  </si>
+  <si>
+    <t>NJD1CGSDIAMOND</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 Retro High OG Bleached Coral, JD1 Trắng Đen Da Nứt</t>
+  </si>
+  <si>
+    <t>NJD1CLOSTNFOUND</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 Retro High OG Lost And Found, JD1 Cao Đỏ Trắng Da Nứt</t>
+  </si>
+  <si>
+    <t>NJD1CPATENTTW</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 Mid Patent Triple White, JD1 Cao Full Trắng</t>
+  </si>
+  <si>
+    <t>NJD1CSATINSH</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 High Satin Shadow Đen Xám Vải Phi</t>
+  </si>
+  <si>
+    <t>NJD1CWHBLP</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 High White Black Cổ Cao Panda Trắng Đen</t>
+  </si>
+  <si>
+    <t>NJD1CWWHTR</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 High White Team Red Cổ Cao Trắng Đỏ Mận</t>
+  </si>
+  <si>
+    <t>NJD1MGREYCAMO</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 Mid Grey Camo, JD1 Mid Xám Camo</t>
+  </si>
+  <si>
+    <t>NJD1TMIDNIGHTNAVY</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 Low Midnight Navy, JD1 Thấp Đen Xanh Than</t>
+  </si>
+  <si>
+    <t>NJD1TNORTHSIDE</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 Low Retro Low North Side, JD1 Thấp Xám Trắng Móc Xanh Rêu</t>
+  </si>
+  <si>
+    <t>NJD1TPWBD</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 Low Panda Black White, JD1 Thấp Đen Trắng Da</t>
+  </si>
+  <si>
+    <t>NJD1TTRIPLEWHITE</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 Low Triple White, JD1 Thấp Full Trắng</t>
+  </si>
+  <si>
+    <t>NJD1TWUNIVSTREDCC</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 Low Thấp Trắng Đỏ Móc Đen, JD1 Low White Univeristy Red</t>
+  </si>
+  <si>
+    <t>NJD1TWWORFGREY</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 1 Low White Wolf Grey, JD1 Thấp Xám Trắng Đế Trong</t>
+  </si>
+  <si>
+    <t>NJD3BLACAT</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 3 Black Cat Full Đen</t>
+  </si>
+  <si>
+    <t>NJD3FRAWHI</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 3 Fragment White Trắng Đen</t>
+  </si>
+  <si>
+    <t>NJD3RAIWOM</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 3 Raised Women Trắng Xám Da Lộn</t>
+  </si>
+  <si>
+    <t>NJD4BREDREIMGN</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Bred Reimagined, JD4 Thấp Đen Viền Đỏ Da</t>
+  </si>
+  <si>
+    <t>NJD4FLINTGREY</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Retro Flint Grey, JD4 Trắng Mũi Xám Da Nhám</t>
+  </si>
+  <si>
+    <t>NJD4FROZENMOMENT</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Retro Frozen Moments, JD4 Xám Full Da Lộn</t>
+  </si>
+  <si>
+    <t>NJD4KAWSGREY</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Kaws Grey, JD4 Xám Full Da Lộn Đế Dạ Quang</t>
+  </si>
+  <si>
+    <t>NJD4MILITARYBLACKC</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Nike SB Military Black Concept, JD4 Trắng Đen Xám</t>
+  </si>
+  <si>
+    <t>NJD4MLTRBW</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Military Black White, JD4 Trắng Đen</t>
+  </si>
+  <si>
+    <t>NJD4PMALLWHITE</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Pure Money All White, JD4 Full Trắng</t>
+  </si>
+  <si>
+    <t>NJD4RBLACKCAT</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Retro Black Cat, JD4 Đen Full</t>
+  </si>
+  <si>
+    <t>NJD4ROGWHCEMENT</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Retro OG White Cement, JD4 Trắng Xám</t>
+  </si>
+  <si>
+    <t>NJD4RSECMOLIVE</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Retro SE Craft Medium Olive, JD4 Xanh Rêu Đen</t>
+  </si>
+  <si>
+    <t>NJD4RTYELLOW BLACK</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Retro Thunder Yellow Black, JD4 Đen Vàng</t>
+  </si>
+  <si>
+    <t>NJD4SBPGREEN</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Retro Nike SB Pine Green, JD4 Trắng Xanh Lá</t>
+  </si>
+  <si>
+    <t>NJD4SEREDTHUNDER</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Retro SE Red Thunder, JD4 Đen Đỏ</t>
+  </si>
+  <si>
+    <t>NJD4SEWHATTHE4</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Retro SE What The 4, JD4 Trắng Đỏ Xanh</t>
+  </si>
+  <si>
+    <t>NJD4TFIRERED</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Fire Red, JD4 Trắng Viền Đỏ</t>
+  </si>
+  <si>
+    <t>NJD4XBT</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 X SB Sapphire White Royal Blue Gum, JD4 Xanh Trắng</t>
+  </si>
+  <si>
+    <t>NJD4XDL</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Jordan 4 Retro SE Craft Photon Dust, JD4 Xám Da Lộn</t>
+  </si>
+  <si>
+    <t>NMAX1BIGRED</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 1 Big Bubble Red Trắng Đỏ</t>
+  </si>
+  <si>
+    <t>NMAX1BLACK</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 1 Black Đen Trắng</t>
+  </si>
+  <si>
+    <t>NMAX1TINT</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 1 Platinum Tint Dark Obsidian Trắng Xám</t>
+  </si>
+  <si>
+    <t>NMAX1WBLACK</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 1 White Black Trắng Đen</t>
+  </si>
+  <si>
+    <t>NMAX1WGUM</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 1 White Gum Trắng Đế Nâu</t>
+  </si>
+  <si>
+    <t>NMAX270STLBO</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 270 Pulse Roam Stone Light Bone Xám Vàng</t>
+  </si>
+  <si>
+    <t>NMAX90CARGOKAKI</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 90 Surplus Cargo Khaki, Air Max 90 Xanh Rêu</t>
+  </si>
+  <si>
+    <t>NMAX97GHOST</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 97 Ghost, Air Max 97 Xám Xanh Min</t>
+  </si>
+  <si>
+    <t>NMAX97OGSBULLET</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 97 OG Silver Bullet, Air Max 97 Xám Trắng Móc Đỏ</t>
+  </si>
+  <si>
+    <t>NMAX97TRIPLEBLACK</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 97 Triple Black, Air Max 97 Đen Full</t>
+  </si>
+  <si>
+    <t>NMAX97TRIPLEWHITE</t>
+  </si>
+  <si>
+    <t>Giày Nike Air Max 97 Triple White Wolf Grey, Air Max 97 Trắng Full</t>
+  </si>
+  <si>
+    <t>NSB58BURGUNDY</t>
+  </si>
+  <si>
+    <t>Giày Nike SB 58 Light Smoke Burgundy Đỏ Xám Da Lộn</t>
+  </si>
+  <si>
+    <t>NSBDPANDASC</t>
+  </si>
+  <si>
+    <t>Giày Nike SB Dunk Panda, SB Panda Đen Trắng</t>
+  </si>
+  <si>
+    <t>NVOME5CAGR</t>
+  </si>
+  <si>
+    <t>Giày Nike Vomero 5 Cangyr Gray Trắng Xám</t>
+  </si>
+  <si>
+    <t>NVOME5GREY</t>
+  </si>
+  <si>
+    <t>Giày Nike Vomero 5 Grey Xám</t>
+  </si>
+  <si>
+    <t>NVOME5PHDME</t>
+  </si>
+  <si>
+    <t>Giày Nike Vomero 5 Photon Dust Metallic Trắng Bạc</t>
+  </si>
+  <si>
+    <t>NVOME5TRBL</t>
+  </si>
+  <si>
+    <t>Giày Nike Vomero 5 Triple Black Full Đen</t>
+  </si>
+  <si>
+    <t>NZLICR</t>
+  </si>
+  <si>
+    <t>Giày Nike zoom Pegasus 35 Light Cream Trắng Kem</t>
+  </si>
+  <si>
+    <t>NZXB</t>
+  </si>
+  <si>
+    <t>Giày Nike Zoom Pegasus 35 Blue, Zoomanh Biển</t>
+  </si>
+  <si>
+    <t>TIGERBLACKWHITE</t>
+  </si>
+  <si>
+    <t>Giày Onitsuka Tiger Tokuten Black White, Tiger Đen Trắng Đế Nâu</t>
+  </si>
+  <si>
+    <t>VANSKNUWBLACK</t>
+  </si>
+  <si>
+    <t>Giày Vans Knu Skool Black White Đen Trắng</t>
+  </si>
+  <si>
+    <t>VANSKNUWGRAY</t>
+  </si>
+  <si>
+    <t>Giày Vans Knu Skool Gray White Xám Trắng</t>
+  </si>
+  <si>
+    <t>VANSKNUWRED</t>
+  </si>
+  <si>
+    <t>Giày Vans Knu Skool White Red Đỏ Trắng</t>
+  </si>
+  <si>
+    <t>YZ350CREAMWHITESC</t>
+  </si>
+  <si>
+    <t>Giày Adidas Yeezy 350 Cream White Full Trắng Hàng Đế Nén Hạt Chuẩn</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1755,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:Q105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="B13" sqref="B13"/>
@@ -1653,10 +1917,10 @@
         <v>26</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I8">
-        <v>315000.0</v>
+        <v>325000.0</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1670,10 +1934,10 @@
         <v>28</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="I9">
-        <v>315000.0</v>
+        <v>325000.0</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1687,10 +1951,10 @@
         <v>30</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I10">
-        <v>315000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1704,10 +1968,10 @@
         <v>32</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I11">
-        <v>415000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1721,10 +1985,10 @@
         <v>34</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I12">
-        <v>415000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1738,10 +2002,10 @@
         <v>36</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I13">
-        <v>415000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1755,10 +2019,10 @@
         <v>38</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I14">
-        <v>415000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1772,10 +2036,10 @@
         <v>40</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I15">
-        <v>415000.0</v>
+        <v>295000.0</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1789,10 +2053,10 @@
         <v>42</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I16">
-        <v>375000.0</v>
+        <v>445000.0</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1806,10 +2070,10 @@
         <v>44</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I17">
-        <v>375000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1823,10 +2087,10 @@
         <v>46</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I18">
-        <v>375000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1840,10 +2104,10 @@
         <v>48</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I19">
-        <v>375000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1857,10 +2121,10 @@
         <v>50</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I20">
-        <v>315000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1874,10 +2138,10 @@
         <v>52</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I21">
-        <v>315000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1891,10 +2155,10 @@
         <v>54</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I22">
-        <v>315000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1908,10 +2172,10 @@
         <v>56</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I23">
-        <v>315000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1925,10 +2189,10 @@
         <v>58</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="I24">
-        <v>315000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1942,10 +2206,10 @@
         <v>60</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I25">
-        <v>315000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1959,7 +2223,7 @@
         <v>62</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I26">
         <v>315000.0</v>
@@ -1976,10 +2240,10 @@
         <v>64</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I27">
-        <v>315000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -1993,10 +2257,10 @@
         <v>66</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I28">
-        <v>395000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2010,10 +2274,10 @@
         <v>68</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I29">
-        <v>395000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2027,10 +2291,10 @@
         <v>70</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="I30">
-        <v>395000.0</v>
+        <v>315000.0</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2044,10 +2308,10 @@
         <v>72</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="I31">
-        <v>395000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -2061,10 +2325,10 @@
         <v>74</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I32">
-        <v>395000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -2078,10 +2342,10 @@
         <v>76</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I33">
-        <v>515000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -2095,10 +2359,10 @@
         <v>78</v>
       </c>
       <c r="D34">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I34">
-        <v>515000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -2112,10 +2376,10 @@
         <v>80</v>
       </c>
       <c r="D35">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="I35">
-        <v>515000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -2129,10 +2393,10 @@
         <v>82</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I36">
-        <v>515000.0</v>
+        <v>465000.0</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -2146,10 +2410,10 @@
         <v>84</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I37">
-        <v>375000.0</v>
+        <v>465000.0</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -2163,10 +2427,10 @@
         <v>86</v>
       </c>
       <c r="D38">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I38">
-        <v>375000.0</v>
+        <v>465000.0</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -2180,10 +2444,10 @@
         <v>88</v>
       </c>
       <c r="D39">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="I39">
-        <v>375000.0</v>
+        <v>495000.0</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -2197,10 +2461,10 @@
         <v>90</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I40">
-        <v>375000.0</v>
+        <v>495000.0</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -2214,10 +2478,10 @@
         <v>92</v>
       </c>
       <c r="D41">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="I41">
-        <v>375000.0</v>
+        <v>365000.0</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -2231,10 +2495,10 @@
         <v>94</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="I42">
-        <v>375000.0</v>
+        <v>365000.0</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -2248,10 +2512,10 @@
         <v>96</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I43">
-        <v>375000.0</v>
+        <v>365000.0</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -2265,10 +2529,10 @@
         <v>98</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I44">
-        <v>375000.0</v>
+        <v>365000.0</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -2282,10 +2546,10 @@
         <v>100</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I45">
-        <v>435000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -2299,10 +2563,10 @@
         <v>102</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I46">
-        <v>435000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -2316,10 +2580,10 @@
         <v>104</v>
       </c>
       <c r="D47">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I47">
-        <v>435000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -2333,10 +2597,10 @@
         <v>106</v>
       </c>
       <c r="D48">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I48">
-        <v>435000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="49" spans="1:17">
@@ -2350,10 +2614,10 @@
         <v>108</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I49">
-        <v>335000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="50" spans="1:17">
@@ -2367,10 +2631,10 @@
         <v>110</v>
       </c>
       <c r="D50">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I50">
-        <v>335000.0</v>
+        <v>465000.0</v>
       </c>
     </row>
     <row r="51" spans="1:17">
@@ -2384,10 +2648,10 @@
         <v>112</v>
       </c>
       <c r="D51">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I51">
-        <v>355000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="52" spans="1:17">
@@ -2401,10 +2665,10 @@
         <v>114</v>
       </c>
       <c r="D52">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I52">
-        <v>355000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="53" spans="1:17">
@@ -2418,10 +2682,10 @@
         <v>116</v>
       </c>
       <c r="D53">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I53">
-        <v>355000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="54" spans="1:17">
@@ -2435,10 +2699,10 @@
         <v>118</v>
       </c>
       <c r="D54">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I54">
-        <v>355000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="55" spans="1:17">
@@ -2452,10 +2716,10 @@
         <v>120</v>
       </c>
       <c r="D55">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I55">
-        <v>355000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="56" spans="1:17">
@@ -2469,10 +2733,10 @@
         <v>122</v>
       </c>
       <c r="D56">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I56">
-        <v>355000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="57" spans="1:17">
@@ -2486,10 +2750,10 @@
         <v>124</v>
       </c>
       <c r="D57">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I57">
-        <v>355000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="58" spans="1:17">
@@ -2503,10 +2767,10 @@
         <v>126</v>
       </c>
       <c r="D58">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I58">
-        <v>355000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="59" spans="1:17">
@@ -2520,10 +2784,10 @@
         <v>128</v>
       </c>
       <c r="D59">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I59">
-        <v>355000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="60" spans="1:17">
@@ -2537,10 +2801,10 @@
         <v>130</v>
       </c>
       <c r="D60">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I60">
-        <v>355000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -2554,10 +2818,758 @@
         <v>132</v>
       </c>
       <c r="D61">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="I61">
-        <v>355000.0</v>
+        <v>345000.0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17">
+      <c r="A62" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" t="s">
+        <v>134</v>
+      </c>
+      <c r="D62">
+        <v>12</v>
+      </c>
+      <c r="I62">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
+      <c r="A63" t="s">
+        <v>135</v>
+      </c>
+      <c r="B63" t="s">
+        <v>135</v>
+      </c>
+      <c r="C63" t="s">
+        <v>136</v>
+      </c>
+      <c r="D63">
+        <v>12</v>
+      </c>
+      <c r="I63">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="A64" t="s">
+        <v>137</v>
+      </c>
+      <c r="B64" t="s">
+        <v>137</v>
+      </c>
+      <c r="C64" t="s">
+        <v>138</v>
+      </c>
+      <c r="D64">
+        <v>12</v>
+      </c>
+      <c r="I64">
+        <v>445000.0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
+      <c r="A65" t="s">
+        <v>139</v>
+      </c>
+      <c r="B65" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" t="s">
+        <v>140</v>
+      </c>
+      <c r="D65">
+        <v>12</v>
+      </c>
+      <c r="I65">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
+      <c r="A66" t="s">
+        <v>141</v>
+      </c>
+      <c r="B66" t="s">
+        <v>141</v>
+      </c>
+      <c r="C66" t="s">
+        <v>142</v>
+      </c>
+      <c r="D66">
+        <v>12</v>
+      </c>
+      <c r="I66">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
+      <c r="A67" t="s">
+        <v>143</v>
+      </c>
+      <c r="B67" t="s">
+        <v>143</v>
+      </c>
+      <c r="C67" t="s">
+        <v>144</v>
+      </c>
+      <c r="D67">
+        <v>12</v>
+      </c>
+      <c r="I67">
+        <v>445000.0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17">
+      <c r="A68" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" t="s">
+        <v>146</v>
+      </c>
+      <c r="D68">
+        <v>12</v>
+      </c>
+      <c r="I68">
+        <v>545000.0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17">
+      <c r="A69" t="s">
+        <v>147</v>
+      </c>
+      <c r="B69" t="s">
+        <v>147</v>
+      </c>
+      <c r="C69" t="s">
+        <v>148</v>
+      </c>
+      <c r="D69">
+        <v>12</v>
+      </c>
+      <c r="I69">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17">
+      <c r="A70" t="s">
+        <v>149</v>
+      </c>
+      <c r="B70" t="s">
+        <v>149</v>
+      </c>
+      <c r="C70" t="s">
+        <v>150</v>
+      </c>
+      <c r="D70">
+        <v>13</v>
+      </c>
+      <c r="I70">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17">
+      <c r="A71" t="s">
+        <v>151</v>
+      </c>
+      <c r="B71" t="s">
+        <v>151</v>
+      </c>
+      <c r="C71" t="s">
+        <v>152</v>
+      </c>
+      <c r="D71">
+        <v>15</v>
+      </c>
+      <c r="I71">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17">
+      <c r="A72" t="s">
+        <v>153</v>
+      </c>
+      <c r="B72" t="s">
+        <v>153</v>
+      </c>
+      <c r="C72" t="s">
+        <v>154</v>
+      </c>
+      <c r="D72">
+        <v>12</v>
+      </c>
+      <c r="I72">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17">
+      <c r="A73" t="s">
+        <v>155</v>
+      </c>
+      <c r="B73" t="s">
+        <v>155</v>
+      </c>
+      <c r="C73" t="s">
+        <v>156</v>
+      </c>
+      <c r="D73">
+        <v>20</v>
+      </c>
+      <c r="I73">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17">
+      <c r="A74" t="s">
+        <v>157</v>
+      </c>
+      <c r="B74" t="s">
+        <v>157</v>
+      </c>
+      <c r="C74" t="s">
+        <v>158</v>
+      </c>
+      <c r="D74">
+        <v>12</v>
+      </c>
+      <c r="I74">
+        <v>445000.0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17">
+      <c r="A75" t="s">
+        <v>159</v>
+      </c>
+      <c r="B75" t="s">
+        <v>159</v>
+      </c>
+      <c r="C75" t="s">
+        <v>160</v>
+      </c>
+      <c r="D75">
+        <v>12</v>
+      </c>
+      <c r="I75">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17">
+      <c r="A76" t="s">
+        <v>161</v>
+      </c>
+      <c r="B76" t="s">
+        <v>161</v>
+      </c>
+      <c r="C76" t="s">
+        <v>162</v>
+      </c>
+      <c r="D76">
+        <v>13</v>
+      </c>
+      <c r="I76">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17">
+      <c r="A77" t="s">
+        <v>163</v>
+      </c>
+      <c r="B77" t="s">
+        <v>163</v>
+      </c>
+      <c r="C77" t="s">
+        <v>164</v>
+      </c>
+      <c r="D77">
+        <v>12</v>
+      </c>
+      <c r="I77">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17">
+      <c r="A78" t="s">
+        <v>165</v>
+      </c>
+      <c r="B78" t="s">
+        <v>165</v>
+      </c>
+      <c r="C78" t="s">
+        <v>166</v>
+      </c>
+      <c r="D78">
+        <v>12</v>
+      </c>
+      <c r="I78">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17">
+      <c r="A79" t="s">
+        <v>167</v>
+      </c>
+      <c r="B79" t="s">
+        <v>167</v>
+      </c>
+      <c r="C79" t="s">
+        <v>168</v>
+      </c>
+      <c r="D79">
+        <v>12</v>
+      </c>
+      <c r="I79">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17">
+      <c r="A80" t="s">
+        <v>169</v>
+      </c>
+      <c r="B80" t="s">
+        <v>169</v>
+      </c>
+      <c r="C80" t="s">
+        <v>170</v>
+      </c>
+      <c r="D80">
+        <v>15</v>
+      </c>
+      <c r="I80">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17">
+      <c r="A81" t="s">
+        <v>171</v>
+      </c>
+      <c r="B81" t="s">
+        <v>171</v>
+      </c>
+      <c r="C81" t="s">
+        <v>172</v>
+      </c>
+      <c r="D81">
+        <v>12</v>
+      </c>
+      <c r="I81">
+        <v>445000.0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17">
+      <c r="A82" t="s">
+        <v>173</v>
+      </c>
+      <c r="B82" t="s">
+        <v>173</v>
+      </c>
+      <c r="C82" t="s">
+        <v>174</v>
+      </c>
+      <c r="D82">
+        <v>12</v>
+      </c>
+      <c r="I82">
+        <v>385000.0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17">
+      <c r="A83" t="s">
+        <v>175</v>
+      </c>
+      <c r="B83" t="s">
+        <v>175</v>
+      </c>
+      <c r="C83" t="s">
+        <v>176</v>
+      </c>
+      <c r="D83">
+        <v>12</v>
+      </c>
+      <c r="I83">
+        <v>385000.0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17">
+      <c r="A84" t="s">
+        <v>177</v>
+      </c>
+      <c r="B84" t="s">
+        <v>177</v>
+      </c>
+      <c r="C84" t="s">
+        <v>178</v>
+      </c>
+      <c r="D84">
+        <v>12</v>
+      </c>
+      <c r="I84">
+        <v>385000.0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17">
+      <c r="A85" t="s">
+        <v>179</v>
+      </c>
+      <c r="B85" t="s">
+        <v>179</v>
+      </c>
+      <c r="C85" t="s">
+        <v>180</v>
+      </c>
+      <c r="D85">
+        <v>18</v>
+      </c>
+      <c r="I85">
+        <v>385000.0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17">
+      <c r="A86" t="s">
+        <v>181</v>
+      </c>
+      <c r="B86" t="s">
+        <v>181</v>
+      </c>
+      <c r="C86" t="s">
+        <v>182</v>
+      </c>
+      <c r="D86">
+        <v>12</v>
+      </c>
+      <c r="I86">
+        <v>385000.0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17">
+      <c r="A87" t="s">
+        <v>183</v>
+      </c>
+      <c r="B87" t="s">
+        <v>183</v>
+      </c>
+      <c r="C87" t="s">
+        <v>184</v>
+      </c>
+      <c r="D87">
+        <v>12</v>
+      </c>
+      <c r="I87">
+        <v>465000.0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17">
+      <c r="A88" t="s">
+        <v>185</v>
+      </c>
+      <c r="B88" t="s">
+        <v>185</v>
+      </c>
+      <c r="C88" t="s">
+        <v>186</v>
+      </c>
+      <c r="D88">
+        <v>12</v>
+      </c>
+      <c r="I88">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17">
+      <c r="A89" t="s">
+        <v>187</v>
+      </c>
+      <c r="B89" t="s">
+        <v>187</v>
+      </c>
+      <c r="C89" t="s">
+        <v>188</v>
+      </c>
+      <c r="D89">
+        <v>12</v>
+      </c>
+      <c r="I89">
+        <v>365000.0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17">
+      <c r="A90" t="s">
+        <v>189</v>
+      </c>
+      <c r="B90" t="s">
+        <v>189</v>
+      </c>
+      <c r="C90" t="s">
+        <v>190</v>
+      </c>
+      <c r="D90">
+        <v>12</v>
+      </c>
+      <c r="I90">
+        <v>365000.0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17">
+      <c r="A91" t="s">
+        <v>191</v>
+      </c>
+      <c r="B91" t="s">
+        <v>191</v>
+      </c>
+      <c r="C91" t="s">
+        <v>192</v>
+      </c>
+      <c r="D91">
+        <v>13</v>
+      </c>
+      <c r="I91">
+        <v>365000.0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17">
+      <c r="A92" t="s">
+        <v>193</v>
+      </c>
+      <c r="B92" t="s">
+        <v>193</v>
+      </c>
+      <c r="C92" t="s">
+        <v>194</v>
+      </c>
+      <c r="D92">
+        <v>13</v>
+      </c>
+      <c r="I92">
+        <v>365000.0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17">
+      <c r="A93" t="s">
+        <v>195</v>
+      </c>
+      <c r="B93" t="s">
+        <v>195</v>
+      </c>
+      <c r="C93" t="s">
+        <v>196</v>
+      </c>
+      <c r="D93">
+        <v>12</v>
+      </c>
+      <c r="I93">
+        <v>385000.0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17">
+      <c r="A94" t="s">
+        <v>197</v>
+      </c>
+      <c r="B94" t="s">
+        <v>197</v>
+      </c>
+      <c r="C94" t="s">
+        <v>198</v>
+      </c>
+      <c r="D94">
+        <v>8</v>
+      </c>
+      <c r="I94">
+        <v>365000.0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17">
+      <c r="A95" t="s">
+        <v>199</v>
+      </c>
+      <c r="B95" t="s">
+        <v>199</v>
+      </c>
+      <c r="C95" t="s">
+        <v>200</v>
+      </c>
+      <c r="D95">
+        <v>12</v>
+      </c>
+      <c r="I95">
+        <v>425000.0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17">
+      <c r="A96" t="s">
+        <v>201</v>
+      </c>
+      <c r="B96" t="s">
+        <v>201</v>
+      </c>
+      <c r="C96" t="s">
+        <v>202</v>
+      </c>
+      <c r="D96">
+        <v>12</v>
+      </c>
+      <c r="I96">
+        <v>425000.0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17">
+      <c r="A97" t="s">
+        <v>203</v>
+      </c>
+      <c r="B97" t="s">
+        <v>203</v>
+      </c>
+      <c r="C97" t="s">
+        <v>204</v>
+      </c>
+      <c r="D97">
+        <v>12</v>
+      </c>
+      <c r="I97">
+        <v>425000.0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17">
+      <c r="A98" t="s">
+        <v>205</v>
+      </c>
+      <c r="B98" t="s">
+        <v>205</v>
+      </c>
+      <c r="C98" t="s">
+        <v>206</v>
+      </c>
+      <c r="D98">
+        <v>6</v>
+      </c>
+      <c r="I98">
+        <v>425000.0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17">
+      <c r="A99" t="s">
+        <v>207</v>
+      </c>
+      <c r="B99" t="s">
+        <v>207</v>
+      </c>
+      <c r="C99" t="s">
+        <v>208</v>
+      </c>
+      <c r="D99">
+        <v>12</v>
+      </c>
+      <c r="I99">
+        <v>385000.0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17">
+      <c r="A100" t="s">
+        <v>209</v>
+      </c>
+      <c r="B100" t="s">
+        <v>209</v>
+      </c>
+      <c r="C100" t="s">
+        <v>210</v>
+      </c>
+      <c r="D100">
+        <v>6</v>
+      </c>
+      <c r="I100">
+        <v>385000.0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17">
+      <c r="A101" t="s">
+        <v>211</v>
+      </c>
+      <c r="B101" t="s">
+        <v>211</v>
+      </c>
+      <c r="C101" t="s">
+        <v>212</v>
+      </c>
+      <c r="D101">
+        <v>12</v>
+      </c>
+      <c r="I101">
+        <v>405000.0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17">
+      <c r="A102" t="s">
+        <v>213</v>
+      </c>
+      <c r="B102" t="s">
+        <v>213</v>
+      </c>
+      <c r="C102" t="s">
+        <v>214</v>
+      </c>
+      <c r="D102">
+        <v>12</v>
+      </c>
+      <c r="I102">
+        <v>385000.0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17">
+      <c r="A103" t="s">
+        <v>215</v>
+      </c>
+      <c r="B103" t="s">
+        <v>215</v>
+      </c>
+      <c r="C103" t="s">
+        <v>216</v>
+      </c>
+      <c r="D103">
+        <v>12</v>
+      </c>
+      <c r="I103">
+        <v>385000.0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17">
+      <c r="A104" t="s">
+        <v>217</v>
+      </c>
+      <c r="B104" t="s">
+        <v>217</v>
+      </c>
+      <c r="C104" t="s">
+        <v>218</v>
+      </c>
+      <c r="D104">
+        <v>12</v>
+      </c>
+      <c r="I104">
+        <v>385000.0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17">
+      <c r="A105" t="s">
+        <v>219</v>
+      </c>
+      <c r="B105" t="s">
+        <v>219</v>
+      </c>
+      <c r="C105" t="s">
+        <v>220</v>
+      </c>
+      <c r="D105">
+        <v>12</v>
+      </c>
+      <c r="I105">
+        <v>405000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix ar and name excel column
</commit_message>
<xml_diff>
--- a/public/uploads/nhap_hang_sapo.xlsx
+++ b/public/uploads/nhap_hang_sapo.xlsx
@@ -580,7 +580,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="201">
   <si>
     <t>Mã đơn nhập</t>
   </si>
@@ -669,12 +669,6 @@
     <t>Giày Nike KillShot 2 Sail Gum Trắng Xám Da Lộn</t>
   </si>
   <si>
-    <t>APUREBTCARBON</t>
-  </si>
-  <si>
-    <t>Giày Adidas Pureboost Carbon, PureBoost Đen Logo Trắng</t>
-  </si>
-  <si>
     <t>APUREBWHITEBLACK</t>
   </si>
   <si>
@@ -699,18 +693,6 @@
     <t>Giày Adidas Samba Pharrell Williams Humanrace Samba Full Kem Da Lộn</t>
   </si>
   <si>
-    <t>ASGL</t>
-  </si>
-  <si>
-    <t>Giày Adidas Superstar Gold Label Superstar Tem Vàng</t>
-  </si>
-  <si>
-    <t>AYMXGREY</t>
-  </si>
-  <si>
-    <t>Giày Adidas Yeezy 350 V2 MX Frost Blue Đen Xám Trắng Hàng Đế Nén Hạt Chuẩn</t>
-  </si>
-  <si>
     <t>AYSLATE</t>
   </si>
   <si>
@@ -723,12 +705,6 @@
     <t>Giày Adidas Yeezy 350 V2 Black Reflective Đen Phản Quang Boost Nén Hạt</t>
   </si>
   <si>
-    <t>AYZ350CINDER</t>
-  </si>
-  <si>
-    <t>Giày Adidas Yeezy 350 V2 Cinder Đen Full</t>
-  </si>
-  <si>
     <t>AYZ350STATICNONTPQ</t>
   </si>
   <si>
@@ -741,24 +717,12 @@
     <t>Giày Adidas Yeezy 350 V2 Lundmark Reflective Kem Xám Boost Nén Hạt</t>
   </si>
   <si>
-    <t>AYZ350V2SESAME</t>
-  </si>
-  <si>
-    <t>Giày Adidas Yeezy 350 V2 Sesame Xám Xi Măng Boost Nén Hạt</t>
-  </si>
-  <si>
     <t>AYZXCW</t>
   </si>
   <si>
     <t>Giày Adidas Yeezy 350 V2 Cloud White Trắng Xanh</t>
   </si>
   <si>
-    <t>MLBCHUNKYWPINK</t>
-  </si>
-  <si>
-    <t>Giày MLB Chunky Liner Denim Monogram NY White Pink Trắng Hồng</t>
-  </si>
-  <si>
     <t>NAF1BGGUM</t>
   </si>
   <si>
@@ -903,12 +867,6 @@
     <t>Giày Nike Air Jordan 1 High Denim Cổ Cao Xanh Jeans</t>
   </si>
   <si>
-    <t>NJD1CGSDIAMOND</t>
-  </si>
-  <si>
-    <t>Giày Nike Air Jordan 1 Retro High OG Bleached Coral, JD1 Trắng Đen Da Nứt</t>
-  </si>
-  <si>
     <t>NJD1CLOSTNFOUND</t>
   </si>
   <si>
@@ -1173,12 +1131,6 @@
     <t>Giày Nike SB 58 Light Smoke Burgundy Đỏ Xám Da Lộn</t>
   </si>
   <si>
-    <t>NSBDPANDASC</t>
-  </si>
-  <si>
-    <t>Giày Nike SB Dunk Panda, SB Panda Đen Trắng</t>
-  </si>
-  <si>
     <t>NVOME5CAGR</t>
   </si>
   <si>
@@ -1197,22 +1149,10 @@
     <t>Giày Nike Vomero 5 Photon Dust Metallic Trắng Bạc</t>
   </si>
   <si>
-    <t>NVOME5TRBL</t>
-  </si>
-  <si>
-    <t>Giày Nike Vomero 5 Triple Black Full Đen</t>
-  </si>
-  <si>
     <t>NZLICR</t>
   </si>
   <si>
     <t>Giày Nike zoom Pegasus 35 Light Cream Trắng Kem</t>
-  </si>
-  <si>
-    <t>NZXB</t>
-  </si>
-  <si>
-    <t>Giày Nike Zoom Pegasus 35 Blue, Zoomanh Biển</t>
   </si>
   <si>
     <t>TIGERBLACKWHITE</t>
@@ -1755,7 +1695,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q105"/>
+  <dimension ref="A1:Q95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="B13" sqref="B13"/>
@@ -1951,7 +1891,7 @@
         <v>30</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I10">
         <v>385000.0</v>
@@ -1985,10 +1925,10 @@
         <v>34</v>
       </c>
       <c r="D12">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I12">
-        <v>385000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -2002,7 +1942,7 @@
         <v>36</v>
       </c>
       <c r="D13">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I13">
         <v>345000.0</v>
@@ -2022,7 +1962,7 @@
         <v>13</v>
       </c>
       <c r="I14">
-        <v>345000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2036,10 +1976,10 @@
         <v>40</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I15">
-        <v>295000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2053,10 +1993,10 @@
         <v>42</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I16">
-        <v>445000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2070,7 +2010,7 @@
         <v>44</v>
       </c>
       <c r="D17">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I17">
         <v>405000.0</v>
@@ -2087,7 +2027,7 @@
         <v>46</v>
       </c>
       <c r="D18">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I18">
         <v>405000.0</v>
@@ -2104,10 +2044,10 @@
         <v>48</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I19">
-        <v>405000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -2121,10 +2061,10 @@
         <v>50</v>
       </c>
       <c r="D20">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I20">
-        <v>405000.0</v>
+        <v>315000.0</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2141,7 +2081,7 @@
         <v>12</v>
       </c>
       <c r="I21">
-        <v>405000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -2155,10 +2095,10 @@
         <v>54</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I22">
-        <v>405000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2189,10 +2129,10 @@
         <v>58</v>
       </c>
       <c r="D24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I24">
-        <v>425000.0</v>
+        <v>315000.0</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -2223,10 +2163,10 @@
         <v>62</v>
       </c>
       <c r="D26">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I26">
-        <v>315000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2243,7 +2183,7 @@
         <v>12</v>
       </c>
       <c r="I27">
-        <v>385000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2257,10 +2197,10 @@
         <v>66</v>
       </c>
       <c r="D28">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I28">
-        <v>385000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2274,7 +2214,7 @@
         <v>68</v>
       </c>
       <c r="D29">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I29">
         <v>405000.0</v>
@@ -2294,7 +2234,7 @@
         <v>12</v>
       </c>
       <c r="I30">
-        <v>315000.0</v>
+        <v>465000.0</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2311,7 +2251,7 @@
         <v>12</v>
       </c>
       <c r="I31">
-        <v>345000.0</v>
+        <v>465000.0</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -2328,7 +2268,7 @@
         <v>12</v>
       </c>
       <c r="I32">
-        <v>345000.0</v>
+        <v>465000.0</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -2345,7 +2285,7 @@
         <v>12</v>
       </c>
       <c r="I33">
-        <v>405000.0</v>
+        <v>495000.0</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -2362,7 +2302,7 @@
         <v>12</v>
       </c>
       <c r="I34">
-        <v>405000.0</v>
+        <v>495000.0</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -2376,10 +2316,10 @@
         <v>80</v>
       </c>
       <c r="D35">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I35">
-        <v>405000.0</v>
+        <v>365000.0</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -2396,7 +2336,7 @@
         <v>12</v>
       </c>
       <c r="I36">
-        <v>465000.0</v>
+        <v>365000.0</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -2410,10 +2350,10 @@
         <v>84</v>
       </c>
       <c r="D37">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I37">
-        <v>465000.0</v>
+        <v>365000.0</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -2427,10 +2367,10 @@
         <v>86</v>
       </c>
       <c r="D38">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I38">
-        <v>465000.0</v>
+        <v>365000.0</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -2447,7 +2387,7 @@
         <v>12</v>
       </c>
       <c r="I39">
-        <v>495000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -2464,7 +2404,7 @@
         <v>12</v>
       </c>
       <c r="I40">
-        <v>495000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -2481,7 +2421,7 @@
         <v>12</v>
       </c>
       <c r="I41">
-        <v>365000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -2498,7 +2438,7 @@
         <v>12</v>
       </c>
       <c r="I42">
-        <v>365000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -2512,10 +2452,10 @@
         <v>96</v>
       </c>
       <c r="D43">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I43">
-        <v>365000.0</v>
+        <v>465000.0</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -2529,10 +2469,10 @@
         <v>98</v>
       </c>
       <c r="D44">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I44">
-        <v>365000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -2549,7 +2489,7 @@
         <v>12</v>
       </c>
       <c r="I45">
-        <v>405000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -2563,7 +2503,7 @@
         <v>102</v>
       </c>
       <c r="D46">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I46">
         <v>425000.0</v>
@@ -2614,10 +2554,10 @@
         <v>108</v>
       </c>
       <c r="D49">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I49">
-        <v>425000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="50" spans="1:17">
@@ -2634,7 +2574,7 @@
         <v>12</v>
       </c>
       <c r="I50">
-        <v>465000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="51" spans="1:17">
@@ -2648,10 +2588,10 @@
         <v>112</v>
       </c>
       <c r="D51">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="I51">
-        <v>425000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="52" spans="1:17">
@@ -2668,7 +2608,7 @@
         <v>12</v>
       </c>
       <c r="I52">
-        <v>425000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="53" spans="1:17">
@@ -2682,10 +2622,10 @@
         <v>116</v>
       </c>
       <c r="D53">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I53">
-        <v>425000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="54" spans="1:17">
@@ -2699,10 +2639,10 @@
         <v>118</v>
       </c>
       <c r="D54">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I54">
-        <v>425000.0</v>
+        <v>345000.0</v>
       </c>
     </row>
     <row r="55" spans="1:17">
@@ -2719,7 +2659,7 @@
         <v>12</v>
       </c>
       <c r="I55">
-        <v>425000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="56" spans="1:17">
@@ -2736,7 +2676,7 @@
         <v>12</v>
       </c>
       <c r="I56">
-        <v>345000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="57" spans="1:17">
@@ -2753,7 +2693,7 @@
         <v>12</v>
       </c>
       <c r="I57">
-        <v>345000.0</v>
+        <v>445000.0</v>
       </c>
     </row>
     <row r="58" spans="1:17">
@@ -2767,10 +2707,10 @@
         <v>126</v>
       </c>
       <c r="D58">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I58">
-        <v>345000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="59" spans="1:17">
@@ -2787,7 +2727,7 @@
         <v>12</v>
       </c>
       <c r="I59">
-        <v>345000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="60" spans="1:17">
@@ -2804,7 +2744,7 @@
         <v>12</v>
       </c>
       <c r="I60">
-        <v>345000.0</v>
+        <v>445000.0</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -2818,10 +2758,10 @@
         <v>132</v>
       </c>
       <c r="D61">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I61">
-        <v>345000.0</v>
+        <v>545000.0</v>
       </c>
     </row>
     <row r="62" spans="1:17">
@@ -2852,7 +2792,7 @@
         <v>136</v>
       </c>
       <c r="D63">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I63">
         <v>405000.0</v>
@@ -2869,10 +2809,10 @@
         <v>138</v>
       </c>
       <c r="D64">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I64">
-        <v>445000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="65" spans="1:17">
@@ -2903,7 +2843,7 @@
         <v>142</v>
       </c>
       <c r="D66">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="I66">
         <v>405000.0</v>
@@ -2940,7 +2880,7 @@
         <v>12</v>
       </c>
       <c r="I68">
-        <v>545000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="69" spans="1:17">
@@ -2954,7 +2894,7 @@
         <v>148</v>
       </c>
       <c r="D69">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I69">
         <v>405000.0</v>
@@ -2971,7 +2911,7 @@
         <v>150</v>
       </c>
       <c r="D70">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I70">
         <v>405000.0</v>
@@ -2988,7 +2928,7 @@
         <v>152</v>
       </c>
       <c r="D71">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I71">
         <v>405000.0</v>
@@ -3022,7 +2962,7 @@
         <v>156</v>
       </c>
       <c r="D73">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I73">
         <v>405000.0</v>
@@ -3059,7 +2999,7 @@
         <v>12</v>
       </c>
       <c r="I75">
-        <v>405000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="76" spans="1:17">
@@ -3073,10 +3013,10 @@
         <v>162</v>
       </c>
       <c r="D76">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I76">
-        <v>405000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="77" spans="1:17">
@@ -3093,7 +3033,7 @@
         <v>12</v>
       </c>
       <c r="I77">
-        <v>405000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="78" spans="1:17">
@@ -3107,10 +3047,10 @@
         <v>166</v>
       </c>
       <c r="D78">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I78">
-        <v>405000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="79" spans="1:17">
@@ -3127,7 +3067,7 @@
         <v>12</v>
       </c>
       <c r="I79">
-        <v>405000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="80" spans="1:17">
@@ -3141,10 +3081,10 @@
         <v>170</v>
       </c>
       <c r="D80">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I80">
-        <v>405000.0</v>
+        <v>465000.0</v>
       </c>
     </row>
     <row r="81" spans="1:17">
@@ -3161,7 +3101,7 @@
         <v>12</v>
       </c>
       <c r="I81">
-        <v>445000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="82" spans="1:17">
@@ -3178,7 +3118,7 @@
         <v>12</v>
       </c>
       <c r="I82">
-        <v>385000.0</v>
+        <v>365000.0</v>
       </c>
     </row>
     <row r="83" spans="1:17">
@@ -3195,7 +3135,7 @@
         <v>12</v>
       </c>
       <c r="I83">
-        <v>385000.0</v>
+        <v>365000.0</v>
       </c>
     </row>
     <row r="84" spans="1:17">
@@ -3209,10 +3149,10 @@
         <v>178</v>
       </c>
       <c r="D84">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I84">
-        <v>385000.0</v>
+        <v>365000.0</v>
       </c>
     </row>
     <row r="85" spans="1:17">
@@ -3226,10 +3166,10 @@
         <v>180</v>
       </c>
       <c r="D85">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I85">
-        <v>385000.0</v>
+        <v>365000.0</v>
       </c>
     </row>
     <row r="86" spans="1:17">
@@ -3263,7 +3203,7 @@
         <v>12</v>
       </c>
       <c r="I87">
-        <v>465000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="88" spans="1:17">
@@ -3280,7 +3220,7 @@
         <v>12</v>
       </c>
       <c r="I88">
-        <v>405000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="89" spans="1:17">
@@ -3297,7 +3237,7 @@
         <v>12</v>
       </c>
       <c r="I89">
-        <v>365000.0</v>
+        <v>425000.0</v>
       </c>
     </row>
     <row r="90" spans="1:17">
@@ -3314,7 +3254,7 @@
         <v>12</v>
       </c>
       <c r="I90">
-        <v>365000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="91" spans="1:17">
@@ -3328,10 +3268,10 @@
         <v>192</v>
       </c>
       <c r="D91">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I91">
-        <v>365000.0</v>
+        <v>405000.0</v>
       </c>
     </row>
     <row r="92" spans="1:17">
@@ -3345,10 +3285,10 @@
         <v>194</v>
       </c>
       <c r="D92">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I92">
-        <v>365000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="93" spans="1:17">
@@ -3379,10 +3319,10 @@
         <v>198</v>
       </c>
       <c r="D94">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I94">
-        <v>365000.0</v>
+        <v>385000.0</v>
       </c>
     </row>
     <row r="95" spans="1:17">
@@ -3399,176 +3339,6 @@
         <v>12</v>
       </c>
       <c r="I95">
-        <v>425000.0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17">
-      <c r="A96" t="s">
-        <v>201</v>
-      </c>
-      <c r="B96" t="s">
-        <v>201</v>
-      </c>
-      <c r="C96" t="s">
-        <v>202</v>
-      </c>
-      <c r="D96">
-        <v>12</v>
-      </c>
-      <c r="I96">
-        <v>425000.0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:17">
-      <c r="A97" t="s">
-        <v>203</v>
-      </c>
-      <c r="B97" t="s">
-        <v>203</v>
-      </c>
-      <c r="C97" t="s">
-        <v>204</v>
-      </c>
-      <c r="D97">
-        <v>12</v>
-      </c>
-      <c r="I97">
-        <v>425000.0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:17">
-      <c r="A98" t="s">
-        <v>205</v>
-      </c>
-      <c r="B98" t="s">
-        <v>205</v>
-      </c>
-      <c r="C98" t="s">
-        <v>206</v>
-      </c>
-      <c r="D98">
-        <v>6</v>
-      </c>
-      <c r="I98">
-        <v>425000.0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:17">
-      <c r="A99" t="s">
-        <v>207</v>
-      </c>
-      <c r="B99" t="s">
-        <v>207</v>
-      </c>
-      <c r="C99" t="s">
-        <v>208</v>
-      </c>
-      <c r="D99">
-        <v>12</v>
-      </c>
-      <c r="I99">
-        <v>385000.0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:17">
-      <c r="A100" t="s">
-        <v>209</v>
-      </c>
-      <c r="B100" t="s">
-        <v>209</v>
-      </c>
-      <c r="C100" t="s">
-        <v>210</v>
-      </c>
-      <c r="D100">
-        <v>6</v>
-      </c>
-      <c r="I100">
-        <v>385000.0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:17">
-      <c r="A101" t="s">
-        <v>211</v>
-      </c>
-      <c r="B101" t="s">
-        <v>211</v>
-      </c>
-      <c r="C101" t="s">
-        <v>212</v>
-      </c>
-      <c r="D101">
-        <v>12</v>
-      </c>
-      <c r="I101">
-        <v>405000.0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:17">
-      <c r="A102" t="s">
-        <v>213</v>
-      </c>
-      <c r="B102" t="s">
-        <v>213</v>
-      </c>
-      <c r="C102" t="s">
-        <v>214</v>
-      </c>
-      <c r="D102">
-        <v>12</v>
-      </c>
-      <c r="I102">
-        <v>385000.0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17">
-      <c r="A103" t="s">
-        <v>215</v>
-      </c>
-      <c r="B103" t="s">
-        <v>215</v>
-      </c>
-      <c r="C103" t="s">
-        <v>216</v>
-      </c>
-      <c r="D103">
-        <v>12</v>
-      </c>
-      <c r="I103">
-        <v>385000.0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:17">
-      <c r="A104" t="s">
-        <v>217</v>
-      </c>
-      <c r="B104" t="s">
-        <v>217</v>
-      </c>
-      <c r="C104" t="s">
-        <v>218</v>
-      </c>
-      <c r="D104">
-        <v>12</v>
-      </c>
-      <c r="I104">
-        <v>385000.0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17">
-      <c r="A105" t="s">
-        <v>219</v>
-      </c>
-      <c r="B105" t="s">
-        <v>219</v>
-      </c>
-      <c r="C105" t="s">
-        <v>220</v>
-      </c>
-      <c r="D105">
-        <v>12</v>
-      </c>
-      <c r="I105">
         <v>405000.0</v>
       </c>
     </row>

</xml_diff>